<commit_message>
$Mi 28. Dez 15:45:51 CET 2022
</commit_message>
<xml_diff>
--- a/python_projects/project_just_for_fun/upwork/expenditure_list.xlsx
+++ b/python_projects/project_just_for_fun/upwork/expenditure_list.xlsx
@@ -11,7 +11,7 @@
     <sheet name="expenditure_sheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">expenditure_sheet!$A$1:$C$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">expenditure_sheet!$B$1:$C$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,35 +25,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">Sr_no</t>
+    <t xml:space="preserve">col1</t>
   </si>
   <si>
     <t xml:space="preserve">xxxxxx</t>
   </si>
   <si>
-    <t xml:space="preserve">related_to</t>
+    <t xml:space="preserve">code</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">beedi jalaye </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">tu meri gf me tera bf</t>
-    </r>
+    <t xml:space="preserve">we  see a miracle next day</t>
   </si>
   <si>
-    <t xml:space="preserve">inder</t>
+    <t xml:space="preserve">we  see miracle next day</t>
   </si>
 </sst>
 </file>
@@ -63,12 +47,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="18">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -84,27 +67,97 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,17 +166,74 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFADD58A"/>
-        <bgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -134,7 +244,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -158,47 +268,115 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFADD58A"/>
@@ -210,7 +388,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -226,7 +404,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -260,12 +438,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.51"/>
@@ -273,7 +451,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -284,24 +462,18 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C2"/>
+  <autoFilter ref="B1:C2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>